<commit_message>
added PCB BOM, added graphs in map to the virginia demo
</commit_message>
<xml_diff>
--- a/amazon_ready_station/station_bom.xlsx
+++ b/amazon_ready_station/station_bom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ArjunTambe/Dropbox/5_AMA/droneiotclient/amazon_ready_station/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4D27431D-01AC-324F-BC79-044F1DC94895}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC5A002-104A-964C-A586-7CBC7EEA5B01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="12800" windowHeight="15500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21300" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="station_bom" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Part</t>
   </si>
@@ -28,18 +28,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>I2C Female Headers</t>
-  </si>
-  <si>
-    <t>ESP Female Headers</t>
-  </si>
-  <si>
-    <t>IR Receiver Female Header</t>
-  </si>
-  <si>
-    <t>Transistor (Logic Inverting)</t>
-  </si>
-  <si>
     <t>Order Link</t>
   </si>
   <si>
@@ -113,12 +101,84 @@
   </si>
   <si>
     <t>SOT-23 package is not widely used; can switch if needed</t>
+  </si>
+  <si>
+    <t>IR LED</t>
+  </si>
+  <si>
+    <t>Resistors, IR LED</t>
+  </si>
+  <si>
+    <t>Resistors, IR Receiver</t>
+  </si>
+  <si>
+    <t>220 Ohm, 0805 package</t>
+  </si>
+  <si>
+    <t>200 Ohm, 0805 package</t>
+  </si>
+  <si>
+    <t>Polarized Capacitor, IR Receiver</t>
+  </si>
+  <si>
+    <t>TSOP382X Photodiode</t>
+  </si>
+  <si>
+    <t>Can pick any part, but make sure frequency matches PWM modulation frequency in the code. Use 382, not 392 (pinouts are different)</t>
+  </si>
+  <si>
+    <t>There is no footprint so you're not limited</t>
+  </si>
+  <si>
+    <t>Tantalum, 1.25 x 1.05mm pads</t>
+  </si>
+  <si>
+    <t>Transistor, logic inverting and 38KHz modulation</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/CR0805-FX-2000ELF/3784732</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/CR0805-FX-2200ELF/3784749</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/avx-corporation/F981C105MMA/4005059</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-semiconductor-opto-division/TSOP38238/1681362</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/osram-opto-semiconductors-inc/SFH-4545/2205955</t>
+  </si>
+  <si>
+    <t>950nm IR emitter</t>
+  </si>
+  <si>
+    <t>950 nm, 38kHz</t>
+  </si>
+  <si>
+    <t>Resistors, LED driver</t>
+  </si>
+  <si>
+    <t>100 Ohm, 0805 package</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RK73G2ATTD1000D/13576043</t>
+  </si>
+  <si>
+    <t>Female Header, IR Receiver</t>
+  </si>
+  <si>
+    <t>Female Headers, ESP</t>
+  </si>
+  <si>
+    <t>Female Headers, I2C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -961,11 +1021,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -975,16 +1035,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -992,16 +1052,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1009,16 +1069,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1026,16 +1086,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1043,19 +1103,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1063,16 +1123,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1080,16 +1140,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1097,16 +1157,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1114,19 +1174,127 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="F9" t="s">
-        <v>29</v>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>